<commit_message>
excel and xml generator modified
</commit_message>
<xml_diff>
--- a/dra_metadata.xlsx
+++ b/dra_metadata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10536" tabRatio="430"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24288" windowHeight="8952" tabRatio="430"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="9" r:id="rId1"/>
@@ -65,7 +65,9 @@
             <family val="3"/>
             <charset val="128"/>
           </rPr>
-          <t>YYYY-MM-DD (e.g, 2024-01-01)</t>
+          <t>YYYY-MM-DD (e.g, 2024-01-01)
+For immediate release, 
+enter date of submission.</t>
         </r>
       </text>
     </comment>
@@ -565,10 +567,6 @@
     <t>AB 310 Genetic Analyzer</t>
   </si>
   <si>
-    <t>v1.0</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>cDNA_randomPriming</t>
   </si>
   <si>
@@ -741,12 +739,16 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>2020-04-08 Bioinformation and DDBJ Center</t>
+    <t>This excel file is used to generate Submission, Experiment and Run XMLs for DDBJ Sequence Read Archive (DRA) submission. 
+Please see https://github.com/ddbj/submission-excel2xml for details.</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>This excel file is used to generate Submission, Experiment and Run XMLs for DDBJ Sequence Read Archive (DRA) submission. 
-Please see https://github.com/ddbj/submission-excel2xml for details.</t>
+    <t>v1.1</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2020-10-09 Bioinformation and DDBJ Center</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -1218,7 +1220,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
@@ -1228,27 +1232,27 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="5" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
     <row r="4" spans="1:1" ht="26.4">
       <c r="A4" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="16" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -1264,7 +1268,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B10"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -1279,24 +1283,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="C1" s="17" t="s">
+    </row>
+    <row r="2" spans="1:3">
+      <c r="C2" s="3"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="16" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="C2" s="3"/>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="16" t="s">
+      <c r="B4" s="16" t="s">
         <v>136</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1344,7 +1348,7 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>9</v>
@@ -1443,7 +1447,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>9</v>
@@ -1480,7 +1484,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>6</v>
@@ -27949,7 +27953,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>28</v>
@@ -27961,7 +27965,7 @@
         <v>30</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>8</v>
@@ -27974,7 +27978,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>33</v>
@@ -27993,7 +27997,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>37</v>
@@ -28006,7 +28010,7 @@
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
@@ -28019,7 +28023,7 @@
         <v>41</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>43</v>
@@ -28056,10 +28060,10 @@
         <v>40</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>48</v>
@@ -28073,10 +28077,10 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>72</v>
@@ -28086,7 +28090,7 @@
       </c>
       <c r="E9" s="10"/>
       <c r="F9" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
@@ -28115,7 +28119,7 @@
         <v>55</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>64</v>
@@ -28128,10 +28132,10 @@
     <row r="12" spans="1:8">
       <c r="A12" s="13"/>
       <c r="B12" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>19</v>
@@ -28144,7 +28148,7 @@
     <row r="13" spans="1:8">
       <c r="A13" s="10"/>
       <c r="B13" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>47</v>
@@ -28160,10 +28164,10 @@
     <row r="14" spans="1:8">
       <c r="A14" s="10"/>
       <c r="B14" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>57</v>
@@ -28176,13 +28180,13 @@
     <row r="15" spans="1:8">
       <c r="A15" s="10"/>
       <c r="B15" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>49</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
@@ -28192,13 +28196,13 @@
     <row r="16" spans="1:8">
       <c r="A16" s="10"/>
       <c r="B16" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>53</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
@@ -28214,7 +28218,7 @@
         <v>56</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
@@ -28240,7 +28244,7 @@
     <row r="19" spans="1:8">
       <c r="A19" s="10"/>
       <c r="B19" s="11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>62</v>
@@ -28256,13 +28260,13 @@
     <row r="20" spans="1:8">
       <c r="A20" s="10"/>
       <c r="B20" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>63</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
@@ -28272,7 +28276,7 @@
     <row r="21" spans="1:8">
       <c r="A21" s="10"/>
       <c r="B21" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>65</v>
@@ -28288,13 +28292,13 @@
     <row r="22" spans="1:8">
       <c r="A22" s="10"/>
       <c r="B22" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>67</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
@@ -28304,13 +28308,13 @@
     <row r="23" spans="1:8">
       <c r="A23" s="10"/>
       <c r="B23" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>4</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
@@ -28320,7 +28324,7 @@
     <row r="24" spans="1:8">
       <c r="A24" s="10"/>
       <c r="B24" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>75</v>
@@ -28342,7 +28346,7 @@
         <v>78</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
@@ -28384,7 +28388,7 @@
     <row r="28" spans="1:8">
       <c r="A28" s="10"/>
       <c r="B28" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>86</v>
@@ -28403,7 +28407,7 @@
         <v>85</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D29" s="10" t="s">
         <v>82</v>
@@ -28475,10 +28479,10 @@
       <c r="A34" s="10"/>
       <c r="B34" s="11"/>
       <c r="C34" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E34" s="10"/>
       <c r="F34" s="10"/>
@@ -28489,10 +28493,10 @@
       <c r="A35" s="10"/>
       <c r="B35" s="11"/>
       <c r="C35" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E35" s="10"/>
       <c r="F35" s="10"/>
@@ -28503,10 +28507,10 @@
       <c r="A36" s="10"/>
       <c r="B36" s="11"/>
       <c r="C36" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
@@ -28556,7 +28560,7 @@
       <c r="B40" s="11"/>
       <c r="C40" s="10"/>
       <c r="D40" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
@@ -28575,12 +28579,12 @@
     </row>
     <row r="43" spans="1:8">
       <c r="D43" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="D44" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -28630,7 +28634,7 @@
     </row>
     <row r="54" spans="4:4">
       <c r="D54" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="55" spans="4:4">

</xml_diff>

<commit_message>
update to xsd 1.5.9
</commit_message>
<xml_diff>
--- a/dra_metadata.xlsx
+++ b/dra_metadata.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.112.22\ykodama\github\submission-excel2xml\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ddbjs4.nig.ac.jp\ykodama\github\submission-excel2xml\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="11820" tabRatio="430"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20124" windowHeight="8772" tabRatio="430"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="9" r:id="rId1"/>
@@ -256,7 +256,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="178">
   <si>
     <t>Library Source</t>
   </si>
@@ -280,9 +280,6 @@
   </si>
   <si>
     <t>MD5 Checksum</t>
-  </si>
-  <si>
-    <t>fastq</t>
   </si>
   <si>
     <t>Title</t>
@@ -728,16 +725,10 @@
     <t>Restriction Digest</t>
   </si>
   <si>
-    <t xml:space="preserve">Illumina MiniSeq      </t>
-  </si>
-  <si>
     <t>5-methylcytidine antibody</t>
   </si>
   <si>
     <t>MBD2 protein methyl-CpG binding domain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NextSeq 550            </t>
   </si>
   <si>
     <t>padlock probes capture method</t>
@@ -762,16 +753,59 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>v1.1</t>
+    <t>BioProject accession</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>2020-11-11 Bioinformation and DDBJ Center</t>
+    <t>2021-07-13 Bioinformation and DDBJ Center</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>BioProject accession</t>
+    <t>v1.2</t>
     <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>NOMe-Seq</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>NextSeq 1000</t>
+  </si>
+  <si>
+    <t>NextSeq 2000</t>
+  </si>
+  <si>
+    <t>NextSeq 550</t>
+  </si>
+  <si>
+    <t>BGISEQ-500</t>
+  </si>
+  <si>
+    <t>DNBSEQ-G400</t>
+  </si>
+  <si>
+    <t>DNBSEQ-T7</t>
+  </si>
+  <si>
+    <t>DNBSEQ-G50</t>
+  </si>
+  <si>
+    <t>MGISEQ-2000RS</t>
+  </si>
+  <si>
+    <t>Sequel II</t>
+  </si>
+  <si>
+    <t>Ion GeneStudio S5</t>
+  </si>
+  <si>
+    <t>Ion GeneStudio S5 plus</t>
+  </si>
+  <si>
+    <t>Ion GeneStudio S5 prime</t>
+  </si>
+  <si>
+    <t>Illumina MiniSeq</t>
   </si>
 </sst>
 </file>
@@ -1243,7 +1277,7 @@
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -1254,27 +1288,27 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="26.4">
       <c r="A4" s="7" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="16" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="18" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -1305,27 +1339,27 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>132</v>
+      <c r="D1" s="16" t="s">
+        <v>161</v>
       </c>
-      <c r="C1" s="17" t="s">
+    </row>
+    <row r="2" spans="1:4">
+      <c r="C2" s="3"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="D1" s="16" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="C2" s="3"/>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="16" t="s">
+      <c r="B4" s="16" t="s">
         <v>135</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1348,9 +1382,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3000" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I3000" sqref="I3000"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
@@ -1373,13 +1407,13 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>2</v>
@@ -1388,28 +1422,28 @@
         <v>0</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G1" s="16" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="J1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="K1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="L1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="16" t="s">
         <v>16</v>
-      </c>
-      <c r="M1" s="16" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1434,21 +1468,21 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Admin!$C$2:$C$37</xm:f>
+            <xm:f>Admin!$E$2:$E$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>J2:J3000</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Admin!$C$2:$C$38</xm:f>
           </x14:formula1>
           <xm:sqref>G2:G3000</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Admin!$D$2:$D$55</xm:f>
+            <xm:f>Admin!$D$2:$D$66</xm:f>
           </x14:formula1>
           <xm:sqref>I2:I3000</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Admin!$E$2:$E$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>J2:J3000</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1474,13 +1508,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1495,9 +1529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4631"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
-    </sheetView>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
   <cols>
@@ -1513,7 +1545,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>6</v>
@@ -27907,7 +27939,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Admin!$F$2:$F$9</xm:f>
+            <xm:f>Admin!$F$2:$F$8</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C3000</xm:sqref>
         </x14:dataValidation>
@@ -27919,9 +27951,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F66" sqref="A1:F66"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
@@ -27941,16 +27975,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F1" s="15" t="s">
         <v>6</v>
@@ -27963,179 +27997,176 @@
         <v>3</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>24</v>
-      </c>
       <c r="E2" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>141</v>
-      </c>
       <c r="F3" s="10" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C4" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="12" t="s">
-        <v>34</v>
-      </c>
       <c r="E4" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>35</v>
+        <v>143</v>
       </c>
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B5" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="D5" s="12" t="s">
         <v>38</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>39</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="10" t="s">
-        <v>144</v>
+        <v>25</v>
       </c>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="10" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="10" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="10" t="s">
-        <v>51</v>
+        <v>147</v>
       </c>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>147</v>
-      </c>
       <c r="C9" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E9" s="10"/>
-      <c r="F9" s="10" t="s">
-        <v>148</v>
-      </c>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
@@ -28145,13 +28176,13 @@
     <row r="11" spans="1:8">
       <c r="A11" s="10"/>
       <c r="B11" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
@@ -28161,13 +28192,13 @@
     <row r="12" spans="1:8">
       <c r="A12" s="13"/>
       <c r="B12" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
@@ -28177,13 +28208,13 @@
     <row r="13" spans="1:8">
       <c r="A13" s="10"/>
       <c r="B13" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
@@ -28193,13 +28224,13 @@
     <row r="14" spans="1:8">
       <c r="A14" s="10"/>
       <c r="B14" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
@@ -28209,13 +28240,13 @@
     <row r="15" spans="1:8">
       <c r="A15" s="10"/>
       <c r="B15" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
@@ -28225,13 +28256,13 @@
     <row r="16" spans="1:8">
       <c r="A16" s="10"/>
       <c r="B16" s="11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
@@ -28241,13 +28272,13 @@
     <row r="17" spans="1:8">
       <c r="A17" s="10"/>
       <c r="B17" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
@@ -28257,13 +28288,13 @@
     <row r="18" spans="1:8">
       <c r="A18" s="10"/>
       <c r="B18" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
@@ -28273,13 +28304,13 @@
     <row r="19" spans="1:8">
       <c r="A19" s="10"/>
       <c r="B19" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
@@ -28289,13 +28320,13 @@
     <row r="20" spans="1:8">
       <c r="A20" s="10"/>
       <c r="B20" s="11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
@@ -28305,13 +28336,13 @@
     <row r="21" spans="1:8">
       <c r="A21" s="10"/>
       <c r="B21" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
@@ -28321,13 +28352,13 @@
     <row r="22" spans="1:8">
       <c r="A22" s="10"/>
       <c r="B22" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
@@ -28337,13 +28368,13 @@
     <row r="23" spans="1:8">
       <c r="A23" s="10"/>
       <c r="B23" s="11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>4</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
@@ -28353,13 +28384,13 @@
     <row r="24" spans="1:8">
       <c r="A24" s="10"/>
       <c r="B24" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
@@ -28369,13 +28400,13 @@
     <row r="25" spans="1:8">
       <c r="A25" s="10"/>
       <c r="B25" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
@@ -28385,13 +28416,13 @@
     <row r="26" spans="1:8">
       <c r="A26" s="10"/>
       <c r="B26" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>73</v>
+        <v>165</v>
       </c>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
@@ -28401,13 +28432,13 @@
     <row r="27" spans="1:8">
       <c r="A27" s="10"/>
       <c r="B27" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>76</v>
+        <v>166</v>
       </c>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
@@ -28417,13 +28448,13 @@
     <row r="28" spans="1:8">
       <c r="A28" s="10"/>
       <c r="B28" s="11" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
@@ -28433,13 +28464,13 @@
     <row r="29" spans="1:8">
       <c r="A29" s="10"/>
       <c r="B29" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
@@ -28449,13 +28480,13 @@
     <row r="30" spans="1:8">
       <c r="A30" s="10"/>
       <c r="B30" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C30" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="C30" s="10" t="s">
-        <v>89</v>
-      </c>
       <c r="D30" s="10" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
@@ -28466,10 +28497,10 @@
       <c r="A31" s="10"/>
       <c r="B31" s="11"/>
       <c r="C31" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
@@ -28479,11 +28510,11 @@
     <row r="32" spans="1:8">
       <c r="A32" s="10"/>
       <c r="B32" s="11"/>
-      <c r="C32" s="10" t="s">
-        <v>93</v>
+      <c r="C32" s="5" t="s">
+        <v>164</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E32" s="10"/>
       <c r="F32" s="10"/>
@@ -28494,10 +28525,10 @@
       <c r="A33" s="10"/>
       <c r="B33" s="11"/>
       <c r="C33" s="10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E33" s="10"/>
       <c r="F33" s="10"/>
@@ -28508,10 +28539,10 @@
       <c r="A34" s="10"/>
       <c r="B34" s="11"/>
       <c r="C34" s="10" t="s">
-        <v>119</v>
+        <v>94</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>125</v>
+        <v>89</v>
       </c>
       <c r="E34" s="10"/>
       <c r="F34" s="10"/>
@@ -28525,7 +28556,7 @@
         <v>118</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>126</v>
+        <v>91</v>
       </c>
       <c r="E35" s="10"/>
       <c r="F35" s="10"/>
@@ -28536,10 +28567,10 @@
       <c r="A36" s="10"/>
       <c r="B36" s="11"/>
       <c r="C36" s="10" t="s">
-        <v>160</v>
+        <v>117</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
@@ -28550,10 +28581,10 @@
       <c r="A37" s="10"/>
       <c r="B37" s="10"/>
       <c r="C37" s="10" t="s">
-        <v>46</v>
+        <v>157</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>94</v>
+        <v>125</v>
       </c>
       <c r="E37" s="10"/>
       <c r="F37" s="10"/>
@@ -28563,9 +28594,11 @@
     <row r="38" spans="1:8">
       <c r="A38" s="10"/>
       <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
+      <c r="C38" s="10" t="s">
+        <v>45</v>
+      </c>
       <c r="D38" s="10" t="s">
-        <v>98</v>
+        <v>126</v>
       </c>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
@@ -28577,7 +28610,7 @@
       <c r="B39" s="11"/>
       <c r="C39" s="10"/>
       <c r="D39" s="10" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
@@ -28589,7 +28622,7 @@
       <c r="B40" s="11"/>
       <c r="C40" s="10"/>
       <c r="D40" s="10" t="s">
-        <v>129</v>
+        <v>168</v>
       </c>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
@@ -28598,77 +28631,132 @@
     </row>
     <row r="41" spans="1:8">
       <c r="D41" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="D42" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="D43" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="D44" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="D45" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="D46" s="10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="D47" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="D48" s="5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4">
+      <c r="D49" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4">
+      <c r="D50" s="5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
-      <c r="D42" s="5" t="s">
+    <row r="51" spans="4:4">
+      <c r="D51" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="52" spans="4:4">
+      <c r="D52" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="53" spans="4:4">
+      <c r="D53" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="54" spans="4:4">
+      <c r="D54" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="55" spans="4:4">
+      <c r="D55" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="56" spans="4:4">
+      <c r="D56" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
-      <c r="D43" s="5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
-      <c r="D44" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="D45" s="5" t="s">
+    <row r="57" spans="4:4">
+      <c r="D57" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
-      <c r="D46" s="5" t="s">
+    <row r="58" spans="4:4">
+      <c r="D58" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
-      <c r="D47" s="5" t="s">
+    <row r="59" spans="4:4">
+      <c r="D59" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
-      <c r="D48" s="5" t="s">
+    <row r="60" spans="4:4">
+      <c r="D60" s="5" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="49" spans="4:4">
-      <c r="D49" s="5" t="s">
+    <row r="61" spans="4:4">
+      <c r="D61" s="5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="50" spans="4:4">
-      <c r="D50" s="5" t="s">
+    <row r="62" spans="4:4">
+      <c r="D62" s="5" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="51" spans="4:4">
-      <c r="D51" s="5" t="s">
-        <v>108</v>
+    <row r="63" spans="4:4">
+      <c r="D63" s="5" t="s">
+        <v>95</v>
       </c>
     </row>
-    <row r="52" spans="4:4">
-      <c r="D52" s="5" t="s">
+    <row r="64" spans="4:4">
+      <c r="D64" s="5" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="53" spans="4:4">
-      <c r="D53" s="5" t="s">
-        <v>97</v>
+    <row r="65" spans="4:4">
+      <c r="D65" s="5" t="s">
+        <v>127</v>
       </c>
     </row>
-    <row r="54" spans="4:4">
-      <c r="D54" s="5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="55" spans="4:4">
-      <c r="D55" s="5" t="s">
-        <v>88</v>
+    <row r="66" spans="4:4">
+      <c r="D66" s="5" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
default cell position improved
</commit_message>
<xml_diff>
--- a/dra_metadata.xlsx
+++ b/dra_metadata.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ykoda\Desktop\submission-excel2xml\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ddbjs4.nig.ac.jp\ykodama\github\submission-excel2xml\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A24405E-03C7-401E-94CE-BE590714BAB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="43728" windowHeight="8940" tabRatio="430"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="9" r:id="rId1"/>
@@ -25,12 +24,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>児玉悠一</author>
   </authors>
   <commentList>
-    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="A6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -50,12 +49,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>児玉悠一</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -72,7 +71,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -87,7 +86,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+    <comment ref="A4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -107,12 +106,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>児玉悠一</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -128,7 +127,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
+    <comment ref="K1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -143,7 +142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
+    <comment ref="L1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -158,7 +157,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -178,12 +177,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>児玉悠一</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -199,7 +198,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -218,12 +217,12 @@
 </file>
 
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>児玉悠一</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -237,7 +236,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000002000000}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -802,18 +801,18 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>2022-078-12 Bioinformation and DDBJ Center</t>
+    <t>v1.3</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>v1.3</t>
+    <t>2022-08-12 Bioinformation and DDBJ Center</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="177" formatCode="0_);\(0\)"/>
@@ -991,8 +990,8 @@
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
-    <cellStyle name="標準 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="標準 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="標準 2" xfId="2"/>
+    <cellStyle name="標準 3" xfId="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="3" builtinId="9"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1275,28 +1274,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="143.1796875" style="5" customWidth="1"/>
-    <col min="2" max="16384" width="8.90625" style="5"/>
+    <col min="1" max="1" width="143.21875" style="5" customWidth="1"/>
+    <col min="2" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="5" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="5" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="25">
+    <row r="4" spans="1:1" ht="26.4">
       <c r="A4" s="7" t="s">
         <v>159</v>
       </c>
@@ -1320,21 +1319,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="14.90625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="2"/>
+    <col min="4" max="4" width="19.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1379,30 +1376,30 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3000" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I3000" sqref="I3000"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="25.90625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="56.81640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.36328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.453125" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.08984375" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.90625" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.08984375" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="65.54296875" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.453125" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.88671875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="56.77734375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="65.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.44140625" style="9" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.36328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.81640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.36328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.90625" style="9"/>
+    <col min="11" max="11" width="14.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.77734375" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -1454,31 +1451,31 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Admin!$A$2:$A$10</xm:f>
           </x14:formula1>
           <xm:sqref>E2:E3000</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Admin!$B$2:$B$30</xm:f>
           </x14:formula1>
           <xm:sqref>F2:F3000</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Admin!$E$2:$E$4</xm:f>
           </x14:formula1>
           <xm:sqref>J2:J3000</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Admin!$C$2:$C$38</xm:f>
           </x14:formula1>
           <xm:sqref>G2:G3000</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000004000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Admin!$D$2:$D$66</xm:f>
           </x14:formula1>
@@ -1491,19 +1488,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
-    </sheetView>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="24.08984375" style="9" customWidth="1"/>
+    <col min="1" max="1" width="24.109375" style="9" customWidth="1"/>
     <col min="2" max="2" width="43" style="9" customWidth="1"/>
-    <col min="3" max="3" width="29.90625" style="9" customWidth="1"/>
-    <col min="4" max="16384" width="8.90625" style="9"/>
+    <col min="3" max="3" width="29.88671875" style="9" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1526,20 +1521,18 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4631"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="41" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.6328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.90625" style="2"/>
+    <col min="2" max="2" width="24.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -27939,7 +27932,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Admin!$F$2:$F$8</xm:f>
           </x14:formula1>
@@ -27952,27 +27945,25 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
-    </sheetView>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="31.6328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.90625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.90625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.08984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.90625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.6328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.90625" style="5"/>
+    <col min="7" max="7" width="21.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13">
+    <row r="1" spans="1:8">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>

</xml_diff>